<commit_message>
Application of working methods in steps
</commit_message>
<xml_diff>
--- a/src/test/testData/PA-testData.xlsx
+++ b/src/test/testData/PA-testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.tanasijevic\IdeaProjects\sCore-Automation\src\test\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rss0105\IdeaProjects\DemoProject\sCore-Automation\src\test\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C83149-BCCB-49AB-AF46-5290B7C0A980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F961C9C-4534-4F9E-BD05-94C1182BFE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="251" xr2:uid="{53FC5945-D556-4F21-A547-DED6371DC1C1}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="251" xr2:uid="{53FC5945-D556-4F21-A547-DED6371DC1C1}"/>
   </bookViews>
   <sheets>
     <sheet name="PA" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Metod plaćanja</t>
   </si>
   <si>
-    <t>Uplata po poilsi</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ugovarač i nosilac osiguranja su isto lice</t>
   </si>
   <si>
@@ -203,6 +200,9 @@
   </si>
   <si>
     <t>20851,00 RSD</t>
+  </si>
+  <si>
+    <t>Uplata po polisi</t>
   </si>
 </sst>
 </file>
@@ -1018,39 +1018,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2774F6C4-36FB-4928-92D9-0ACED8594BC6}">
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.26953125" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.90625" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.453125" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7265625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="18.26953125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.08984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.36328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.77734375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.36328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.90625" style="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.453125" style="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.81640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.90625" style="1"/>
+    <col min="19" max="19" width="12.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J1" s="50" t="s">
         <v>15</v>
@@ -1091,39 +1091,39 @@
         <v>21</v>
       </c>
       <c r="N1" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O1" s="53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P1" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R1" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="56" t="s">
+      <c r="T1" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="57" t="s">
-        <v>33</v>
-      </c>
       <c r="U1" s="60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V1" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>6</v>
@@ -1147,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="33" t="s">
         <v>16</v>
@@ -1159,42 +1159,42 @@
         <v>20</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="N2" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="36" t="s">
-        <v>25</v>
-      </c>
       <c r="P2" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="39" t="s">
-        <v>30</v>
-      </c>
       <c r="S2" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="40" t="s">
-        <v>35</v>
-      </c>
       <c r="U2" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V2" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W2" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>6</v>
@@ -1212,13 +1212,13 @@
         <v>10</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="33" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="33" t="s">
         <v>16</v>
@@ -1230,42 +1230,42 @@
         <v>20</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="N3" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="36" t="s">
-        <v>25</v>
-      </c>
       <c r="P3" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="39" t="s">
-        <v>30</v>
-      </c>
       <c r="S3" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="40" t="s">
-        <v>35</v>
-      </c>
       <c r="U3" s="61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V3" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W3" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>6</v>
@@ -1283,13 +1283,13 @@
         <v>10</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="33" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="33" t="s">
         <v>16</v>
@@ -1301,42 +1301,42 @@
         <v>20</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="N4" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="36" t="s">
-        <v>25</v>
-      </c>
       <c r="P4" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="39" t="s">
-        <v>30</v>
-      </c>
       <c r="S4" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="40" t="s">
-        <v>35</v>
-      </c>
       <c r="U4" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V4" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W4" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>6</v>
@@ -1354,13 +1354,13 @@
         <v>10</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="33" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" s="33" t="s">
         <v>16</v>
@@ -1372,40 +1372,40 @@
         <v>20</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="N5" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="36" t="s">
-        <v>25</v>
-      </c>
       <c r="P5" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q5" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="39" t="s">
-        <v>30</v>
-      </c>
       <c r="S5" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T5" s="40" t="s">
-        <v>35</v>
-      </c>
       <c r="U5" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V5" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W5" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -1430,7 +1430,7 @@
       <c r="V6" s="22"/>
       <c r="W6" s="24"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -1455,7 +1455,7 @@
       <c r="V7" s="22"/>
       <c r="W7" s="24"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -1480,7 +1480,7 @@
       <c r="V8" s="22"/>
       <c r="W8" s="24"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -1505,7 +1505,7 @@
       <c r="V9" s="22"/>
       <c r="W9" s="24"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -1530,7 +1530,7 @@
       <c r="V10" s="22"/>
       <c r="W10" s="24"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -1555,7 +1555,7 @@
       <c r="V11" s="22"/>
       <c r="W11" s="24"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -1580,7 +1580,7 @@
       <c r="V12" s="22"/>
       <c r="W12" s="24"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -1605,7 +1605,7 @@
       <c r="V13" s="22"/>
       <c r="W13" s="24"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -1630,7 +1630,7 @@
       <c r="V14" s="22"/>
       <c r="W14" s="24"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -1655,7 +1655,7 @@
       <c r="V15" s="22"/>
       <c r="W15" s="24"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -1680,7 +1680,7 @@
       <c r="V16" s="22"/>
       <c r="W16" s="24"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -1705,7 +1705,7 @@
       <c r="V17" s="22"/>
       <c r="W17" s="24"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -1730,7 +1730,7 @@
       <c r="V18" s="22"/>
       <c r="W18" s="24"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -1755,7 +1755,7 @@
       <c r="V19" s="22"/>
       <c r="W19" s="24"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -1780,7 +1780,7 @@
       <c r="V20" s="22"/>
       <c r="W20" s="24"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -1805,7 +1805,7 @@
       <c r="V21" s="22"/>
       <c r="W21" s="24"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -1830,7 +1830,7 @@
       <c r="V22" s="22"/>
       <c r="W22" s="24"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -1855,7 +1855,7 @@
       <c r="V23" s="22"/>
       <c r="W23" s="24"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -1880,7 +1880,7 @@
       <c r="V24" s="22"/>
       <c r="W24" s="24"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -1905,7 +1905,7 @@
       <c r="V25" s="22"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
@@ -1930,7 +1930,7 @@
       <c r="V26" s="22"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -1955,7 +1955,7 @@
       <c r="V27" s="22"/>
       <c r="W27" s="24"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -1980,7 +1980,7 @@
       <c r="V28" s="22"/>
       <c r="W28" s="24"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -2005,7 +2005,7 @@
       <c r="V29" s="22"/>
       <c r="W29" s="24"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -2030,7 +2030,7 @@
       <c r="V30" s="22"/>
       <c r="W30" s="24"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -2055,7 +2055,7 @@
       <c r="V31" s="22"/>
       <c r="W31" s="24"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -2080,7 +2080,7 @@
       <c r="V32" s="22"/>
       <c r="W32" s="24"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -2105,7 +2105,7 @@
       <c r="V33" s="22"/>
       <c r="W33" s="24"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -2130,7 +2130,7 @@
       <c r="V34" s="22"/>
       <c r="W34" s="24"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
@@ -2155,7 +2155,7 @@
       <c r="V35" s="22"/>
       <c r="W35" s="24"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -2180,7 +2180,7 @@
       <c r="V36" s="22"/>
       <c r="W36" s="24"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
@@ -2205,7 +2205,7 @@
       <c r="V37" s="22"/>
       <c r="W37" s="24"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -2230,7 +2230,7 @@
       <c r="V38" s="22"/>
       <c r="W38" s="24"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -2255,7 +2255,7 @@
       <c r="V39" s="22"/>
       <c r="W39" s="24"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -2280,7 +2280,7 @@
       <c r="V40" s="22"/>
       <c r="W40" s="24"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
@@ -2305,7 +2305,7 @@
       <c r="V41" s="22"/>
       <c r="W41" s="24"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -2330,7 +2330,7 @@
       <c r="V42" s="22"/>
       <c r="W42" s="24"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
@@ -2355,7 +2355,7 @@
       <c r="V43" s="22"/>
       <c r="W43" s="24"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
@@ -2380,7 +2380,7 @@
       <c r="V44" s="22"/>
       <c r="W44" s="24"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
@@ -2405,7 +2405,7 @@
       <c r="V45" s="22"/>
       <c r="W45" s="24"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
@@ -2430,7 +2430,7 @@
       <c r="V46" s="22"/>
       <c r="W46" s="24"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
@@ -2455,7 +2455,7 @@
       <c r="V47" s="22"/>
       <c r="W47" s="24"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -2480,7 +2480,7 @@
       <c r="V48" s="22"/>
       <c r="W48" s="24"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
@@ -2505,7 +2505,7 @@
       <c r="V49" s="22"/>
       <c r="W49" s="24"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -2530,7 +2530,7 @@
       <c r="V50" s="22"/>
       <c r="W50" s="24"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
@@ -2555,7 +2555,7 @@
       <c r="V51" s="22"/>
       <c r="W51" s="24"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
@@ -2580,7 +2580,7 @@
       <c r="V52" s="22"/>
       <c r="W52" s="24"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
@@ -2605,7 +2605,7 @@
       <c r="V53" s="22"/>
       <c r="W53" s="24"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
@@ -2630,7 +2630,7 @@
       <c r="V54" s="22"/>
       <c r="W54" s="24"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
@@ -2655,7 +2655,7 @@
       <c r="V55" s="22"/>
       <c r="W55" s="24"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
@@ -2680,7 +2680,7 @@
       <c r="V56" s="22"/>
       <c r="W56" s="24"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
@@ -2705,7 +2705,7 @@
       <c r="V57" s="22"/>
       <c r="W57" s="24"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
@@ -2730,7 +2730,7 @@
       <c r="V58" s="22"/>
       <c r="W58" s="24"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="7"/>
       <c r="C59" s="8"/>
@@ -2755,7 +2755,7 @@
       <c r="V59" s="22"/>
       <c r="W59" s="24"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
@@ -2780,7 +2780,7 @@
       <c r="V60" s="22"/>
       <c r="W60" s="24"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
@@ -2805,7 +2805,7 @@
       <c r="V61" s="22"/>
       <c r="W61" s="24"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
@@ -2830,7 +2830,7 @@
       <c r="V62" s="22"/>
       <c r="W62" s="24"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
@@ -2855,7 +2855,7 @@
       <c r="V63" s="22"/>
       <c r="W63" s="24"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
@@ -2880,7 +2880,7 @@
       <c r="V64" s="22"/>
       <c r="W64" s="24"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
@@ -2905,7 +2905,7 @@
       <c r="V65" s="22"/>
       <c r="W65" s="24"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
@@ -2930,7 +2930,7 @@
       <c r="V66" s="22"/>
       <c r="W66" s="24"/>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
@@ -2955,7 +2955,7 @@
       <c r="V67" s="22"/>
       <c r="W67" s="24"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
@@ -2980,7 +2980,7 @@
       <c r="V68" s="22"/>
       <c r="W68" s="24"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
@@ -3005,7 +3005,7 @@
       <c r="V69" s="22"/>
       <c r="W69" s="24"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
@@ -3030,7 +3030,7 @@
       <c r="V70" s="22"/>
       <c r="W70" s="24"/>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
@@ -3055,7 +3055,7 @@
       <c r="V71" s="22"/>
       <c r="W71" s="24"/>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
@@ -3080,7 +3080,7 @@
       <c r="V72" s="22"/>
       <c r="W72" s="24"/>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
@@ -3105,7 +3105,7 @@
       <c r="V73" s="22"/>
       <c r="W73" s="24"/>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
@@ -3130,7 +3130,7 @@
       <c r="V74" s="22"/>
       <c r="W74" s="24"/>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
@@ -3155,7 +3155,7 @@
       <c r="V75" s="22"/>
       <c r="W75" s="24"/>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
@@ -3180,7 +3180,7 @@
       <c r="V76" s="22"/>
       <c r="W76" s="24"/>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
@@ -3205,7 +3205,7 @@
       <c r="V77" s="22"/>
       <c r="W77" s="24"/>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
@@ -3230,7 +3230,7 @@
       <c r="V78" s="22"/>
       <c r="W78" s="24"/>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
@@ -3255,7 +3255,7 @@
       <c r="V79" s="22"/>
       <c r="W79" s="24"/>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
@@ -3280,7 +3280,7 @@
       <c r="V80" s="22"/>
       <c r="W80" s="24"/>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -3305,7 +3305,7 @@
       <c r="V81" s="22"/>
       <c r="W81" s="24"/>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3330,7 +3330,7 @@
       <c r="V82" s="22"/>
       <c r="W82" s="24"/>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3355,7 +3355,7 @@
       <c r="V83" s="22"/>
       <c r="W83" s="24"/>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3380,7 +3380,7 @@
       <c r="V84" s="22"/>
       <c r="W84" s="24"/>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -3405,7 +3405,7 @@
       <c r="V85" s="22"/>
       <c r="W85" s="24"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -3430,7 +3430,7 @@
       <c r="V86" s="22"/>
       <c r="W86" s="24"/>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
@@ -3455,7 +3455,7 @@
       <c r="V87" s="22"/>
       <c r="W87" s="24"/>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
@@ -3480,7 +3480,7 @@
       <c r="V88" s="22"/>
       <c r="W88" s="24"/>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>

</xml_diff>

<commit_message>
correction in all classes by name
</commit_message>
<xml_diff>
--- a/src/test/testData/PA-testData.xlsx
+++ b/src/test/testData/PA-testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rss0105\IdeaProjects\DemoProject\sCore-Automation\src\test\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F961C9C-4534-4F9E-BD05-94C1182BFE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7182FF-963A-4E18-86B2-D04CA98C59E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="251" xr2:uid="{53FC5945-D556-4F21-A547-DED6371DC1C1}"/>
   </bookViews>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2774F6C4-36FB-4928-92D9-0ACED8594BC6}">
   <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>